<commit_message>
update plots with general instead of synonyms
</commit_message>
<xml_diff>
--- a/bib_data/1990-2017/cluster_distance.xlsx
+++ b/bib_data/1990-2017/cluster_distance.xlsx
@@ -366,13 +366,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -394,11 +394,8 @@
       <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -423,11 +420,8 @@
       <c r="H2">
         <v>2.120864197530864</v>
       </c>
-      <c r="I2">
-        <v>2.233333333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -452,11 +446,8 @@
       <c r="H3">
         <v>1.941045321637427</v>
       </c>
-      <c r="I3">
-        <v>2.230994152046784</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -481,11 +472,8 @@
       <c r="H4">
         <v>2.093826219512195</v>
       </c>
-      <c r="I4">
-        <v>2.63719512195122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -510,11 +498,8 @@
       <c r="H5">
         <v>2.796127450980392</v>
       </c>
-      <c r="I5">
-        <v>3.147058823529412</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -539,11 +524,8 @@
       <c r="H6">
         <v>2.391340361445783</v>
       </c>
-      <c r="I6">
-        <v>2.656626506024097</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -568,11 +550,8 @@
       <c r="H7">
         <v>2.169405594405594</v>
       </c>
-      <c r="I7">
-        <v>2.555944055944056</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -596,38 +575,6 @@
       </c>
       <c r="H8">
         <v>1.2325</v>
-      </c>
-      <c r="I8">
-        <v>2.475</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>2.233333333333333</v>
-      </c>
-      <c r="C9">
-        <v>2.230994152046784</v>
-      </c>
-      <c r="D9">
-        <v>2.63719512195122</v>
-      </c>
-      <c r="E9">
-        <v>3.147058823529412</v>
-      </c>
-      <c r="F9">
-        <v>2.656626506024097</v>
-      </c>
-      <c r="G9">
-        <v>2.555944055944056</v>
-      </c>
-      <c r="H9">
-        <v>2.475</v>
-      </c>
-      <c r="I9">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>